<commit_message>
Added a parsedSheet type in order to limit the amount of reads on the file itself
</commit_message>
<xml_diff>
--- a/parse/data/data.xlsx
+++ b/parse/data/data.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="9015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="9015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ONE_FIRST_CELL" sheetId="1" r:id="rId1"/>
     <sheet name="ONE_DATE" sheetId="2" r:id="rId2"/>
+    <sheet name="PARSE" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +23,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>jkl</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -351,7 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -381,4 +408,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.1111</v>
+      </c>
+      <c r="D2" s="2">
+        <f ca="1">TODAY()</f>
+        <v>44145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1.2330000000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D4" ca="1" si="0">TODAY()</f>
+        <v>44145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3.24342</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>